<commit_message>
Entrega final del tp
</commit_message>
<xml_diff>
--- a/TP1/links.xlsx
+++ b/TP1/links.xlsx
@@ -478,35 +478,35 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//deportes/futbol/asi-quedo-el-cuadro-de-la-copa-argentina-2024-tras-el-triunfo-de-boca-nid24032024/</t>
+          <t>https://www.lanacion.com.ar//politica/javier-milei-en-vivo-las-ultimas-medidas-del-gobierno-nid23032024/</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/el-consumidor-paga-fortunas-el-productor-cobra-migajas-nid24032024/</t>
+          <t>https://www.lanacion.com.ar//politica/javier-milei-y-fatima-florez-fueron-al-teatro-y-cantaron-euforicos-canciones-de-sandro-nid24032024/</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/las-rampas-de-acceso-y-las-cajas-transparentes-como-sigue-la-pelicula-de-la-inteligencia-artificial-nid24032024/</t>
+          <t>https://www.lanacion.com.ar//deportes/futbol/asi-quedo-el-cuadro-de-la-copa-argentina-2024-tras-el-triunfo-de-boca-nid24032024/</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//autos/electricos/que-hara-que-la-economia-argentina-vuelva-a-crecer-nid24032024/</t>
+          <t>https://www.lanacion.com.ar//economia/el-consumidor-paga-fortunas-el-productor-cobra-migajas-nid24032024/</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//economia/un-nuevo-proyecto-de-ganancias-que-no-resuelve-la-cuestion-de-fondo-nid24032024/</t>
+          <t>https://www.lanacion.com.ar//economia/las-rampas-de-acceso-y-las-cajas-transparentes-como-sigue-la-pelicula-de-la-inteligencia-artificial-nid24032024/</t>
         </is>
       </c>
     </row>
@@ -576,7 +576,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//politica/javier-milei-en-vivo-las-ultimas-medidas-del-gobierno-nid23032024/</t>
+          <t>https://www.lanacion.com.ar//politica/javier-milei-y-fatima-florez-fueron-al-teatro-y-cantaron-euforicos-canciones-de-sandro-nid24032024/</t>
         </is>
       </c>
     </row>
@@ -1010,35 +1010,35 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//seguridad/millonario-robo-en-palermo-entro-a-un-local-amenazo-a-los-empleados-con-un-arma-los-encerro-y-se-nid23032024/</t>
+          <t>https://www.lanacion.com.ar//politica/marcha-por-el-24-de-marzo-la-izquierda-el-kirchnerismo-y-grupos-de-derechos-humanos-se-movilizan-nid23032024/</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//politica/lamento-que-scioli-haya-recibido-cifras-falsas-para-tomar-su-decision-nid23032024/</t>
+          <t>https://www.lanacion.com.ar//politica/posse-extiende-su-influencia-a-la-afi-y-advierten-sobre-el-regreso-de-viejas-practicas-en-el-area-de-nid23032024/</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//espectaculos/teatro/en-fotos-los-famosos-disfrutaron-del-estreno-de-mejor-no-decirlo-la-obra-de-mercedes-moran-e-imanol-nid23032024/</t>
+          <t>https://www.lanacion.com.ar//economia/como-quedarian-los-haberes-jubilatorios-de-la-anses-en-abril-nid23032024/</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//el-mundo/atentado-en-moscu-por-que-putin-apunta-contra-ucrania-y-no-menciona-a-estado-islamico-nid23032024/</t>
+          <t>https://www.lanacion.com.ar//seguridad/los-videos-claves-que-incriminan-a-la-empleada-domestica-del-ingeniero-asesinado-en-el-country-la-nid23032024/</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar//politica/el-intercambio-entre-javier-milei-y-victoria-villarruel-tras-la-marcha-en-contra-de-la-ley-de-aborto-nid23032024/</t>
+          <t>https://www.lanacion.com.ar//el-mundo/la-historia-del-despiadado-comerciante-de-esclavos-que-dio-su-nombre-a-una-de-las-universidades-mas-nid23032024/</t>
         </is>
       </c>
     </row>

</xml_diff>